<commit_message>
update world cup template
</commit_message>
<xml_diff>
--- a/extra/excel_templates/WorldCup_2026.xlsx
+++ b/extra/excel_templates/WorldCup_2026.xlsx
@@ -11,7 +11,6 @@
     <sheet name="Matches" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Countries" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Groups" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Stadiums" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="314">
   <si>
     <t xml:space="preserve">Country 1</t>
   </si>
@@ -49,13 +48,16 @@
     <t xml:space="preserve">GROUP_A</t>
   </si>
   <si>
-    <t xml:space="preserve">Mexico City Stadium, Mexico City</t>
+    <t xml:space="preserve">Mexico City Stadium</t>
   </si>
   <si>
     <t xml:space="preserve">KOREA_REPUBLIC</t>
   </si>
   <si>
-    <t xml:space="preserve">Estadio Guadalajara, Guadalajara (MEX)</t>
+    <t xml:space="preserve">noch offen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estadio Guadalajara</t>
   </si>
   <si>
     <t xml:space="preserve">CANADA</t>
@@ -64,7 +66,7 @@
     <t xml:space="preserve">GROUP_B</t>
   </si>
   <si>
-    <t xml:space="preserve">Toronto-Stadion, Toronto (CA)</t>
+    <t xml:space="preserve">Toronto-Stadion</t>
   </si>
   <si>
     <t xml:space="preserve">USA</t>
@@ -76,7 +78,7 @@
     <t xml:space="preserve">GROUP_D</t>
   </si>
   <si>
-    <t xml:space="preserve">Los Angeles Stadium, Los Angeles (USA)</t>
+    <t xml:space="preserve">Los Angeles Stadium</t>
   </si>
   <si>
     <t xml:space="preserve">QATAR</t>
@@ -85,7 +87,7 @@
     <t xml:space="preserve">SWITZERLAND</t>
   </si>
   <si>
-    <t xml:space="preserve">San Francisco Bay Area Stadium, San Francisco Bay Area (USA)</t>
+    <t xml:space="preserve">San Francisco Bay</t>
   </si>
   <si>
     <t xml:space="preserve">BRAZIL</t>
@@ -97,7 +99,7 @@
     <t xml:space="preserve">GROUP_C</t>
   </si>
   <si>
-    <t xml:space="preserve">New York New Jersey Stadium, New York/New Jersey (USA)</t>
+    <t xml:space="preserve">New York New Jersey</t>
   </si>
   <si>
     <t xml:space="preserve">HAITI</t>
@@ -106,13 +108,13 @@
     <t xml:space="preserve">SCOTLAND</t>
   </si>
   <si>
-    <t xml:space="preserve">Boston Stadium, Boston (USA)</t>
+    <t xml:space="preserve">Boston Stadium</t>
   </si>
   <si>
     <t xml:space="preserve">AUSTRALIA</t>
   </si>
   <si>
-    <t xml:space="preserve">Vancouver-Stadion, Vancouver (CA)</t>
+    <t xml:space="preserve">Vancouver-Stadion</t>
   </si>
   <si>
     <t xml:space="preserve">GERMANY</t>
@@ -124,7 +126,7 @@
     <t xml:space="preserve">GROUP_E</t>
   </si>
   <si>
-    <t xml:space="preserve">Houston Stadium, Houston (USA)</t>
+    <t xml:space="preserve">Houston Stadium</t>
   </si>
   <si>
     <t xml:space="preserve">NETHERLANDS</t>
@@ -136,7 +138,7 @@
     <t xml:space="preserve">GROUP_F</t>
   </si>
   <si>
-    <t xml:space="preserve">Dallas Stadium, Dallas (USA)</t>
+    <t xml:space="preserve">Dallas Stadium</t>
   </si>
   <si>
     <t xml:space="preserve">IVORY_COAST</t>
@@ -145,13 +147,13 @@
     <t xml:space="preserve">ECUADOR</t>
   </si>
   <si>
-    <t xml:space="preserve">Philadelphia Stadium, Philadelphia (USA)</t>
+    <t xml:space="preserve">Philadelphia Stadium</t>
   </si>
   <si>
     <t xml:space="preserve">TUNISIA</t>
   </si>
   <si>
-    <t xml:space="preserve">Estadio Monterrey, Monterrey (MEX)</t>
+    <t xml:space="preserve">Estadio Monterrey</t>
   </si>
   <si>
     <t xml:space="preserve">SPAIN</t>
@@ -163,7 +165,7 @@
     <t xml:space="preserve">GROUP_H</t>
   </si>
   <si>
-    <t xml:space="preserve">Atlanta Stadium, Atlanta (USA)</t>
+    <t xml:space="preserve">Atlanta Stadium</t>
   </si>
   <si>
     <t xml:space="preserve">BELGIUM</t>
@@ -175,7 +177,7 @@
     <t xml:space="preserve">GROUP_G</t>
   </si>
   <si>
-    <t xml:space="preserve">Seattle Stadium, Seattle (USA)</t>
+    <t xml:space="preserve">Seattle Stadium</t>
   </si>
   <si>
     <t xml:space="preserve">SAUDI_ARABIA</t>
@@ -184,7 +186,7 @@
     <t xml:space="preserve">URUGUAY</t>
   </si>
   <si>
-    <t xml:space="preserve">Miami Stadium, Miami (USA)</t>
+    <t xml:space="preserve">Miami Stadium</t>
   </si>
   <si>
     <t xml:space="preserve">IRAN</t>
@@ -214,7 +216,7 @@
     <t xml:space="preserve">GROUP_J</t>
   </si>
   <si>
-    <t xml:space="preserve">Kansas City Stadium, Kansas City (USA)</t>
+    <t xml:space="preserve">Kansas City Stadium</t>
   </si>
   <si>
     <t xml:space="preserve">AUSTRIA</t>
@@ -248,9 +250,6 @@
   </si>
   <si>
     <t xml:space="preserve">COLOMBIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mexico City Stadium, Mexico City (MEX)</t>
   </si>
   <si>
     <t xml:space="preserve">Zweiter Gruppe A</t>
@@ -971,9 +970,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -1055,7 +1055,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1069,6 +1069,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1160,7 +1164,7 @@
   <dimension ref="A1:E440"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1169,10 +1173,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="18.45"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1189,7 +1193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1202,391 +1206,405 @@
       <c r="D2" s="3" t="n">
         <v>46184.875</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>46185.1666666667</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>46185.875</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>46186.125</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>46186.875</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" s="3" t="n">
         <v>46187</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D8" s="3" t="n">
         <v>46187.125</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3" t="n">
         <v>46187.25</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" s="3" t="n">
         <v>46187.7916666667</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3" t="n">
         <v>46187.9166666667</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" s="3" t="n">
         <v>46188.0416666667</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
+      <c r="E12" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B13" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13" s="3" t="n">
         <v>46188.1666666667</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D14" s="3" t="n">
         <v>46188.75</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E14" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D15" s="3" t="n">
         <v>46188.875</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>46189</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>46189</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="4" t="n">
+      <c r="D17" s="5" t="n">
         <v>46189.125</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="4" t="n">
+        <v>59</v>
+      </c>
+      <c r="D18" s="5" t="n">
         <v>46189.875</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2"/>
+      <c r="E18" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="4" t="n">
+      <c r="D19" s="5" t="n">
         <v>46190</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="4" t="n">
+        <v>63</v>
+      </c>
+      <c r="D20" s="5" t="n">
         <v>46190.125</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="4" t="n">
+      <c r="D21" s="5" t="n">
         <v>46190.25</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C22" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="4" t="n">
+        <v>68</v>
+      </c>
+      <c r="D22" s="5" t="n">
         <v>46190.7916666667</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="4" t="n">
+        <v>71</v>
+      </c>
+      <c r="D23" s="5" t="n">
         <v>46190.9166666667</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="D24" s="3" t="n">
         <v>46191.0416666667</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D25" s="3" t="n">
         <v>46191.1666666667</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2"/>
+      <c r="E25" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B26" s="2" t="s">
         <v>6</v>
       </c>
@@ -1596,43 +1614,45 @@
       <c r="D26" s="3" t="n">
         <v>46191.75</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C27" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D27" s="3" t="n">
         <v>46191.875</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="D28" s="6" t="n">
         <v>46192</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>5</v>
       </c>
@@ -1642,413 +1662,425 @@
       <c r="C29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="5" t="n">
+      <c r="D29" s="6" t="n">
         <v>46192.125</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="6" t="n">
+        <v>45827.875</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="6" t="n">
+        <v>46193</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="6" t="n">
+        <v>46193.125</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+      <c r="B33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="6" t="n">
+        <v>46193.25</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="6" t="n">
+        <v>46193.7916666667</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="6" t="n">
+        <v>46193.9166666667</v>
+      </c>
+      <c r="E35" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="5" t="n">
-        <v>45827.875</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="5" t="n">
-        <v>46193</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="5" t="n">
-        <v>46193.125</v>
-      </c>
-      <c r="E32" s="2" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="5" t="n">
-        <v>46193.25</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="5" t="n">
-        <v>46193.7916666667</v>
-      </c>
-      <c r="E34" s="2" t="s">
+      <c r="B36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="5" t="n">
-        <v>46193.9166666667</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D36" s="3" t="n">
         <v>46194.0833333333</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D37" s="3" t="n">
         <v>46194.25</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D38" s="3" t="n">
         <v>46194.75</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D39" s="3" t="n">
         <v>46194.875</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D40" s="3" t="n">
         <v>46195</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D41" s="3" t="n">
         <v>46195.125</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E41" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D42" s="3" t="n">
         <v>46195.7916666667</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E42" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C43" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D43" s="3" t="n">
         <v>46195.9583333333</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E43" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="D44" s="3" t="n">
         <v>46196.0833333333</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E44" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D45" s="3" t="n">
         <v>46196.2083333333</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E45" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D46" s="3" t="n">
         <v>46196.7916666667</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E46" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="D47" s="3" t="n">
         <v>46196.9166666667</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E47" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D48" s="3" t="n">
         <v>46197.0416666667</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E48" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B49" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C49" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D49" s="3" t="n">
         <v>46197.1666666667</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D50" s="3" t="n">
         <v>46197.875</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2"/>
+      <c r="E50" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B51" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D51" s="3" t="n">
         <v>46197.875</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D52" s="3" t="n">
         <v>46198</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D53" s="3" t="n">
         <v>46198</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2"/>
+      <c r="E53" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B54" s="2" t="s">
         <v>5</v>
       </c>
@@ -2058,11 +2090,11 @@
       <c r="D54" s="3" t="n">
         <v>46198.125</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E54" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
         <v>6</v>
       </c>
@@ -2075,306 +2107,314 @@
       <c r="D55" s="3" t="n">
         <v>46198.125</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E55" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D56" s="3" t="n">
         <v>46198.9166666667</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E56" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="B57" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D57" s="3" t="n">
         <v>46198.9166666667</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E57" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B58" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C58" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D58" s="3" t="n">
         <v>46199.0416666667</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E58" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="D59" s="3" t="n">
         <v>46199.0416666667</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="2"/>
+      <c r="E59" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B60" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D60" s="3" t="n">
         <v>46199.1666666667</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E60" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="D61" s="3" t="n">
         <v>46199.1666666667</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E61" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="D62" s="3" t="n">
         <v>46199.875</v>
       </c>
-      <c r="E62" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E62" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B63" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C63" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D63" s="3" t="n">
         <v>46199.875</v>
       </c>
-      <c r="E63" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E63" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D64" s="3" t="n">
         <v>46200.0833333333</v>
       </c>
-      <c r="E64" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E64" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D65" s="3" t="n">
         <v>46200.0833333333</v>
       </c>
-      <c r="E65" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E65" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D66" s="3" t="n">
         <v>46200.2083333333</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="E66" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="D67" s="3" t="n">
         <v>46200.2083333333</v>
       </c>
-      <c r="E67" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E67" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D68" s="3" t="n">
         <v>46200.9583333333</v>
       </c>
-      <c r="E68" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E68" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="D69" s="3" t="n">
         <v>46200.9583333333</v>
       </c>
-      <c r="E69" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E69" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D70" s="3" t="n">
         <v>46201.0625</v>
       </c>
-      <c r="E70" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2"/>
+      <c r="E70" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B71" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D71" s="3" t="n">
         <v>46201.0625</v>
       </c>
-      <c r="E71" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E71" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D72" s="3" t="n">
         <v>46201.1666666667</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="E72" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="D73" s="3" t="n">
         <v>46201.1666666667</v>
       </c>
-      <c r="E73" s="2" t="s">
-        <v>37</v>
+      <c r="E73" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2390,8 +2430,8 @@
       <c r="D74" s="3" t="n">
         <v>46201.875</v>
       </c>
-      <c r="E74" s="2" t="s">
-        <v>17</v>
+      <c r="E74" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2407,8 +2447,8 @@
       <c r="D75" s="3" t="n">
         <v>46202.7916666667</v>
       </c>
-      <c r="E75" s="2" t="s">
-        <v>33</v>
+      <c r="E75" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2424,8 +2464,8 @@
       <c r="D76" s="3" t="n">
         <v>46202.9375</v>
       </c>
-      <c r="E76" s="2" t="s">
-        <v>27</v>
+      <c r="E76" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2441,8 +2481,8 @@
       <c r="D77" s="3" t="n">
         <v>46203.125</v>
       </c>
-      <c r="E77" s="2" t="s">
-        <v>42</v>
+      <c r="E77" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2458,8 +2498,8 @@
       <c r="D78" s="3" t="n">
         <v>46203.7916666667</v>
       </c>
-      <c r="E78" s="2" t="s">
-        <v>37</v>
+      <c r="E78" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,8 +2515,8 @@
       <c r="D79" s="3" t="n">
         <v>46203.9583333333</v>
       </c>
-      <c r="E79" s="2" t="s">
-        <v>24</v>
+      <c r="E79" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2492,8 +2532,8 @@
       <c r="D80" s="3" t="n">
         <v>46204.125</v>
       </c>
-      <c r="E80" s="2" t="s">
-        <v>75</v>
+      <c r="E80" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2509,8 +2549,8 @@
       <c r="D81" s="3" t="n">
         <v>46204.75</v>
       </c>
-      <c r="E81" s="2" t="s">
-        <v>46</v>
+      <c r="E81" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2526,8 +2566,8 @@
       <c r="D82" s="3" t="n">
         <v>46204.9166666667</v>
       </c>
-      <c r="E82" s="2" t="s">
-        <v>50</v>
+      <c r="E82" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2543,8 +2583,8 @@
       <c r="D83" s="3" t="n">
         <v>46205.0833333333</v>
       </c>
-      <c r="E83" s="2" t="s">
-        <v>20</v>
+      <c r="E83" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2560,8 +2600,8 @@
       <c r="D84" s="3" t="n">
         <v>46205.875</v>
       </c>
-      <c r="E84" s="2" t="s">
-        <v>17</v>
+      <c r="E84" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2577,8 +2617,8 @@
       <c r="D85" s="3" t="n">
         <v>46206.0416666667</v>
       </c>
-      <c r="E85" s="2" t="s">
-        <v>13</v>
+      <c r="E85" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,8 +2634,8 @@
       <c r="D86" s="3" t="n">
         <v>46206.2083333333</v>
       </c>
-      <c r="E86" s="2" t="s">
-        <v>29</v>
+      <c r="E86" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2611,8 +2651,8 @@
       <c r="D87" s="3" t="n">
         <v>46206.8333333333</v>
       </c>
-      <c r="E87" s="2" t="s">
-        <v>37</v>
+      <c r="E87" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2628,8 +2668,8 @@
       <c r="D88" s="3" t="n">
         <v>46207</v>
       </c>
-      <c r="E88" s="2" t="s">
-        <v>53</v>
+      <c r="E88" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2645,11 +2685,11 @@
       <c r="D89" s="3" t="n">
         <v>46207.1458333333</v>
       </c>
-      <c r="E89" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E89" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
         <v>109</v>
       </c>
@@ -2662,11 +2702,11 @@
       <c r="D90" s="3" t="n">
         <v>46207.7916666667</v>
       </c>
-      <c r="E90" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E90" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
         <v>112</v>
       </c>
@@ -2679,11 +2719,11 @@
       <c r="D91" s="3" t="n">
         <v>46207.9583333333</v>
       </c>
-      <c r="E91" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E91" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
         <v>114</v>
       </c>
@@ -2696,11 +2736,11 @@
       <c r="D92" s="3" t="n">
         <v>46208.9166666667</v>
       </c>
-      <c r="E92" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E92" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
         <v>116</v>
       </c>
@@ -2713,11 +2753,11 @@
       <c r="D93" s="3" t="n">
         <v>46209.0833333333</v>
       </c>
-      <c r="E93" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E93" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
         <v>118</v>
       </c>
@@ -2730,11 +2770,11 @@
       <c r="D94" s="3" t="n">
         <v>46209.875</v>
       </c>
-      <c r="E94" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E94" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
         <v>120</v>
       </c>
@@ -2747,11 +2787,11 @@
       <c r="D95" s="3" t="n">
         <v>46210.0833333333</v>
       </c>
-      <c r="E95" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E95" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
         <v>122</v>
       </c>
@@ -2764,11 +2804,11 @@
       <c r="D96" s="3" t="n">
         <v>46210.75</v>
       </c>
-      <c r="E96" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E96" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
         <v>124</v>
       </c>
@@ -2781,11 +2821,11 @@
       <c r="D97" s="3" t="n">
         <v>46210.9166666667</v>
       </c>
-      <c r="E97" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E97" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
         <v>126</v>
       </c>
@@ -2798,11 +2838,11 @@
       <c r="D98" s="3" t="n">
         <v>46212.9166666667</v>
       </c>
-      <c r="E98" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E98" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
         <v>129</v>
       </c>
@@ -2815,11 +2855,11 @@
       <c r="D99" s="3" t="n">
         <v>46213.875</v>
       </c>
-      <c r="E99" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E99" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
         <v>131</v>
       </c>
@@ -2832,11 +2872,11 @@
       <c r="D100" s="3" t="n">
         <v>46214.9583333333</v>
       </c>
-      <c r="E100" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E100" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
         <v>133</v>
       </c>
@@ -2849,11 +2889,11 @@
       <c r="D101" s="3" t="n">
         <v>46215.125</v>
       </c>
-      <c r="E101" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E101" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
         <v>135</v>
       </c>
@@ -2866,11 +2906,11 @@
       <c r="D102" s="3" t="n">
         <v>46217.875</v>
       </c>
-      <c r="E102" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E102" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="s">
         <v>138</v>
       </c>
@@ -2883,11 +2923,11 @@
       <c r="D103" s="3" t="n">
         <v>46218.875</v>
       </c>
-      <c r="E103" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E103" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
         <v>140</v>
       </c>
@@ -2900,11 +2940,11 @@
       <c r="D104" s="3" t="n">
         <v>46221.9583333333</v>
       </c>
-      <c r="E104" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E104" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
         <v>143</v>
       </c>
@@ -2917,8 +2957,8 @@
       <c r="D105" s="3" t="n">
         <v>46222.875</v>
       </c>
-      <c r="E105" s="2" t="s">
-        <v>24</v>
+      <c r="E105" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4978,8 +5018,8 @@
       <formula1>Groups!$A$1:$A$18</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E142" type="list">
-      <formula1>Stadiums!$A:$A</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E106:E142" type="list">
+      <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -5021,7 +5061,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5051,7 +5091,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5066,12 +5106,12 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5106,7 +5146,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5146,7 +5186,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5186,12 +5226,12 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5226,7 +5266,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5256,7 +5296,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5266,7 +5306,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5301,12 +5341,12 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5316,7 +5356,7 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5356,7 +5396,7 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5376,12 +5416,12 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5431,7 +5471,7 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5461,7 +5501,7 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5486,7 +5526,7 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5496,12 +5536,12 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5661,7 +5701,7 @@
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5686,7 +5726,7 @@
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5696,7 +5736,7 @@
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5721,7 +5761,7 @@
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5741,7 +5781,7 @@
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5751,7 +5791,7 @@
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5771,7 +5811,7 @@
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5781,7 +5821,7 @@
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5816,17 +5856,17 @@
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5881,7 +5921,7 @@
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5926,7 +5966,7 @@
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5976,7 +6016,7 @@
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6011,7 +6051,7 @@
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6021,12 +6061,12 @@
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6078,7 +6118,7 @@
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6093,57 +6133,57 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6174,113 +6214,6 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>142</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A16"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.66"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>